<commit_message>
atualização modelos arc e iia
</commit_message>
<xml_diff>
--- a/ml_lab/data/td_arc.xlsx
+++ b/ml_lab/data/td_arc.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="357">
   <si>
     <t>Feature</t>
   </si>
@@ -1022,13 +1022,74 @@
   </si>
   <si>
     <t>O valor da consulta muda dependendo do horário?</t>
+  </si>
+  <si>
+    <t>Quero agendar uma consulta</t>
+  </si>
+  <si>
+    <t>Eu gostaria de agendar uma consulta para meu filho</t>
+  </si>
+  <si>
+    <t>Você não atende depois das 17:00 hrs né ?</t>
+  </si>
+  <si>
+    <t>Qual horário vc tem disponível ? Dia 04/03</t>
+  </si>
+  <si>
+    <t>Pode ser no dia 07/03</t>
+  </si>
+  <si>
+    <t>E no dia 12/03 tem horário disponível ?</t>
+  </si>
+  <si>
+    <t>Ele sai da escola 17:30 teria que ser depois desse horário</t>
+  </si>
+  <si>
+    <t>O endereço é esse que está no WhatsApp ?</t>
+  </si>
+  <si>
+    <t>Então eu queria saber o valor da limpeza? Pq aí já agendava a consulta</t>
+  </si>
+  <si>
+    <t>Infantil</t>
+  </si>
+  <si>
+    <t>Tá , qual dia tem horário ?</t>
+  </si>
+  <si>
+    <t>Limpeza , queria para o dia 10 de março</t>
+  </si>
+  <si>
+    <t>Está confirmado amanhã às 08 horas?</t>
+  </si>
+  <si>
+    <t>Daqui a pouco estou ai</t>
+  </si>
+  <si>
+    <t>Bom dia Eni a tia não tá bem tô com muita tosse queria que vc marca se pra outro dia a minha visita aí desculpa beijos 😔</t>
+  </si>
+  <si>
+    <t>Fui tô tomando remédio obrigada</t>
+  </si>
+  <si>
+    <t>Estou precisando fazer uma limpeza pesada kkkkkk 
+ Saiu minha contenção dos dentes de baixo e está até com tártaro 🙆🏻‍♀️</t>
+  </si>
+  <si>
+    <t>Qual seu último horário de atendimento</t>
+  </si>
+  <si>
+    <t>Quebrou um dente 😞</t>
+  </si>
+  <si>
+    <t>Gostaria de agendar um horário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1048,6 +1109,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1063,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1077,6 +1143,12 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1295,7 +1367,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.0"/>
+    <col customWidth="1" min="1" max="1" width="157.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4658,6 +4730,166 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="421">
+      <c r="A421" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B421" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B422" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B423" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B424" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B425" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B426" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B427" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B428" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B429" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B430" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B431" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B432" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B433" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B434" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B435" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B436" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B437" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B438" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B439" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B440" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>